<commit_message>
final version of vrpb.py
</commit_message>
<xml_diff>
--- a/excels/experiment.xlsx
+++ b/excels/experiment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micky\Desktop\wing's stuff\TUD\yr 4\q1\Operations and Optimisations\ops group proj\code\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9A5ADE-AFEA-449C-B4FD-F0A857B183A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D81832-ECA6-42C6-A6E7-F99F9AA8C5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="4872" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -887,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:E201"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,10 +915,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="D2">
         <v>0</v>

</xml_diff>